<commit_message>
Trimmer fix, BOM done
</commit_message>
<xml_diff>
--- a/kk_sem_ultrahang_hw_bom.xlsx
+++ b/kk_sem_ultrahang_hw_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balazs\Documents\git\kk-sem-ultrahang-hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BDFA993-33A7-4BAC-B444-9EB6C3FBBB6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD8AC0-8D41-4486-ABBD-7C1449185EDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{81796AB7-53DE-480E-97DB-C5D69645F3D3}"/>
   </bookViews>
@@ -33,9 +33,317 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t>VALUE</t>
+  </si>
+  <si>
+    <t>PACKAGE</t>
+  </si>
+  <si>
+    <t>PART</t>
+  </si>
+  <si>
+    <t>NOTE</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>SUPPLYER</t>
+  </si>
+  <si>
+    <t>ORDER QTY</t>
+  </si>
+  <si>
+    <t>PRICE (HUF)</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>DIODE</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>CRYSTAL</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>CAPACITOR</t>
+  </si>
+  <si>
+    <t>100n-50V</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>X7R</t>
+  </si>
+  <si>
+    <t>X5R</t>
+  </si>
+  <si>
+    <t>22p-50V</t>
+  </si>
+  <si>
+    <t>C0G</t>
+  </si>
+  <si>
+    <t>10n-50V</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>RESISTOR</t>
+  </si>
+  <si>
+    <t>1% 1/8W</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>5% 1/8W</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>FUSE</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>THT</t>
+  </si>
+  <si>
+    <t>2.54mm, vertical</t>
+  </si>
+  <si>
+    <t>PCB QTY</t>
+  </si>
+  <si>
+    <t>TL974ID</t>
+  </si>
+  <si>
+    <t>SOIC-14</t>
+  </si>
+  <si>
+    <t>U1, U2</t>
+  </si>
+  <si>
+    <t>STM32F070F6P6</t>
+  </si>
+  <si>
+    <t>TSSOP-20</t>
+  </si>
+  <si>
+    <t>LD1117S33TR</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>LD1117S18TR</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SMAJ5.0A</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>8M</t>
+  </si>
+  <si>
+    <t>1n-50V</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5, C6, C8, C9, C10, C11</t>
+  </si>
+  <si>
+    <t>C7, C13, C16, C20, C22, C24</t>
+  </si>
+  <si>
+    <t>C12, C17</t>
+  </si>
+  <si>
+    <t>C14, C21, C23, C25</t>
+  </si>
+  <si>
+    <t>10u-16V</t>
+  </si>
+  <si>
+    <t>1u-16V</t>
+  </si>
+  <si>
+    <t>C18, C19</t>
+  </si>
+  <si>
+    <t>C0G 1%</t>
+  </si>
+  <si>
+    <t>1210</t>
+  </si>
+  <si>
+    <t>50mA PTC</t>
+  </si>
+  <si>
+    <t>3p socket header</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>5p pin header</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>USB 2.0 Mini-B</t>
+  </si>
+  <si>
+    <t>R1, R11</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R12, R15, R19</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>VR1</t>
+  </si>
+  <si>
+    <t>Bourns 3314G</t>
+  </si>
+  <si>
+    <t>16k</t>
+  </si>
+  <si>
+    <t>27k</t>
+  </si>
+  <si>
+    <t>39k</t>
+  </si>
+  <si>
+    <t>2k4</t>
+  </si>
+  <si>
+    <t>6k8</t>
+  </si>
+  <si>
+    <t>2k7</t>
+  </si>
+  <si>
+    <t>1k1</t>
+  </si>
+  <si>
+    <t>820</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>91k</t>
+  </si>
+  <si>
+    <t>620</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>1k6</t>
+  </si>
+  <si>
+    <t>6k2</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,16 +352,82 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -61,17 +435,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -381,12 +801,941 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291FD758-5D1A-4BF4-8D9E-99A6B71ACB77}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.9296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="6">
+        <f>$M$1*2</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="6">
+        <f t="shared" ref="A8" si="0">$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" s="6">
+        <f t="shared" ref="A11" si="1">$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" s="5"/>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" s="6">
+        <f>$M$1*10</f>
+        <v>10</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" s="6">
+        <f>$M$1*6</f>
+        <v>6</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" s="6">
+        <f>$M$1*2</f>
+        <v>2</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" s="6">
+        <f>$M$1*4</f>
+        <v>4</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" s="6">
+        <f>$M$1*2</f>
+        <v>2</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" s="5"/>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" s="6">
+        <f>$M$1*2</f>
+        <v>2</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" s="6">
+        <f t="shared" ref="A20:A36" si="2">$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A22" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A24" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A25" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" s="6">
+        <f>$M$1*3</f>
+        <v>3</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" s="5"/>
+      <c r="B37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" s="5"/>
+      <c r="B39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A40" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A41" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" s="6">
+        <f>$M$1*1</f>
+        <v>1</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <conditionalFormatting sqref="J1:J42">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",J1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Ordered">
+      <formula>NOT(ISERROR(SEARCH("Ordered",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J6 J8:J9 J11 J13:J18 J20:J36 J38 J40:J42" xr:uid="{F7F205F8-AFB0-4666-BB5B-48C0AB512A47}">
+      <formula1>"Ordered,Done"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
C12 changed to 100nF
</commit_message>
<xml_diff>
--- a/kk_sem_ultrahang_hw_bom.xlsx
+++ b/kk_sem_ultrahang_hw_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balazs\Documents\git\kk-sem-ultrahang-hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD8AC0-8D41-4486-ABBD-7C1449185EDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FFCF8A-C3AF-4CBD-8388-52DBF05513F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{81796AB7-53DE-480E-97DB-C5D69645F3D3}"/>
   </bookViews>
@@ -198,12 +198,6 @@
     <t>C1, C2, C3, C4, C5, C6, C8, C9, C10, C11</t>
   </si>
   <si>
-    <t>C7, C13, C16, C20, C22, C24</t>
-  </si>
-  <si>
-    <t>C12, C17</t>
-  </si>
-  <si>
     <t>C14, C21, C23, C25</t>
   </si>
   <si>
@@ -337,6 +331,12 @@
   </si>
   <si>
     <t>1k</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C7, C12, C13, C16, C20, C22, C24</t>
   </si>
 </sst>
 </file>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291FD758-5D1A-4BF4-8D9E-99A6B71ACB77}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1077,7 +1077,7 @@
         <v>53</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
@@ -1087,8 +1087,8 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
-        <f>$M$1*6</f>
-        <v>6</v>
+        <f>$M$1*7</f>
+        <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>21</v>
@@ -1097,7 +1097,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>23</v>
@@ -1110,8 +1110,8 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
-        <f>$M$1*2</f>
-        <v>2</v>
+        <f>$M$1*1</f>
+        <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>27</v>
@@ -1120,7 +1120,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>23</v>
@@ -1137,13 +1137,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>24</v>
@@ -1160,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>22</v>
@@ -1189,7 +1189,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>26</v>
@@ -1220,13 +1220,13 @@
         <v>2</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>30</v>
@@ -1239,11 +1239,11 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
-        <f t="shared" ref="A20:A36" si="2">$M$1*1</f>
+        <f t="shared" ref="A21:A36" si="2">$M$1*1</f>
         <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>22</v>
@@ -1266,13 +1266,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>30</v>
@@ -1289,13 +1289,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>30</v>
@@ -1312,13 +1312,13 @@
         <v>1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>30</v>
@@ -1335,13 +1335,13 @@
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>30</v>
@@ -1358,13 +1358,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>30</v>
@@ -1381,13 +1381,13 @@
         <v>1</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>30</v>
@@ -1404,13 +1404,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>30</v>
@@ -1427,13 +1427,13 @@
         <v>1</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>30</v>
@@ -1450,13 +1450,13 @@
         <v>3</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>30</v>
@@ -1473,13 +1473,13 @@
         <v>1</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>30</v>
@@ -1496,13 +1496,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>30</v>
@@ -1519,13 +1519,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>30</v>
@@ -1542,13 +1542,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>30</v>
@@ -1571,7 +1571,7 @@
         <v>22</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>32</v>
@@ -1594,10 +1594,10 @@
         <v>18</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
@@ -1625,10 +1625,10 @@
         <v>1</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>35</v>
@@ -1660,13 +1660,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>38</v>
@@ -1683,13 +1683,13 @@
         <v>1</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>38</v>
@@ -1706,13 +1706,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="7"/>

</xml_diff>

<commit_message>
Added MIC 100nF, U2D ref
</commit_message>
<xml_diff>
--- a/kk_sem_ultrahang_hw_bom.xlsx
+++ b/kk_sem_ultrahang_hw_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balazs\Documents\git\kk-sem-ultrahang-hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FFCF8A-C3AF-4CBD-8388-52DBF05513F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71EF750-AE6D-46E8-B3E9-1551728E25B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{81796AB7-53DE-480E-97DB-C5D69645F3D3}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>10n-50V</t>
   </si>
   <si>
-    <t>C15</t>
-  </si>
-  <si>
     <t>RESISTOR</t>
   </si>
   <si>
@@ -195,21 +192,12 @@
     <t>1n-50V</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C6, C8, C9, C10, C11</t>
-  </si>
-  <si>
-    <t>C14, C21, C23, C25</t>
-  </si>
-  <si>
     <t>10u-16V</t>
   </si>
   <si>
     <t>1u-16V</t>
   </si>
   <si>
-    <t>C18, C19</t>
-  </si>
-  <si>
     <t>C0G 1%</t>
   </si>
   <si>
@@ -333,10 +321,22 @@
     <t>1k</t>
   </si>
   <si>
-    <t>C17</t>
-  </si>
-  <si>
-    <t>C7, C12, C13, C16, C20, C22, C24</t>
+    <t>C1, C2, C3, C4, C5, C6, C9, C10, C11, C12</t>
+  </si>
+  <si>
+    <t>C7, C8, C13, C14, C17, C21, C23, C25</t>
+  </si>
+  <si>
+    <t>C15, C22, C24, C26</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19, C20</t>
   </si>
 </sst>
 </file>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291FD758-5D1A-4BF4-8D9E-99A6B71ACB77}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -812,7 +812,7 @@
     <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.46484375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.06640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -853,7 +853,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M1" s="10">
         <v>1</v>
@@ -879,13 +879,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
@@ -900,10 +900,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>11</v>
@@ -921,10 +921,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>12</v>
@@ -942,13 +942,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
@@ -977,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>22</v>
@@ -998,7 +998,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>14</v>
@@ -1033,7 +1033,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>18</v>
@@ -1068,16 +1068,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
@@ -1087,8 +1087,8 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
-        <f>$M$1*7</f>
-        <v>7</v>
+        <f>$M$1*8</f>
+        <v>8</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>21</v>
@@ -1097,7 +1097,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>23</v>
@@ -1114,16 +1114,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
@@ -1137,16 +1137,16 @@
         <v>4</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
@@ -1160,13 +1160,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>23</v>
@@ -1189,7 +1189,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>26</v>
@@ -1203,7 +1203,7 @@
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="5"/>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1220,16 +1220,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
@@ -1243,16 +1243,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
@@ -1266,16 +1266,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
@@ -1289,16 +1289,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
@@ -1312,16 +1312,16 @@
         <v>1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
@@ -1335,16 +1335,16 @@
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
@@ -1358,16 +1358,16 @@
         <v>1</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
@@ -1381,16 +1381,16 @@
         <v>1</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
@@ -1404,16 +1404,16 @@
         <v>1</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
@@ -1427,16 +1427,16 @@
         <v>1</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
@@ -1450,16 +1450,16 @@
         <v>3</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
@@ -1473,16 +1473,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
@@ -1496,16 +1496,16 @@
         <v>1</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
@@ -1519,16 +1519,16 @@
         <v>1</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
@@ -1542,16 +1542,16 @@
         <v>1</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
@@ -1565,16 +1565,16 @@
         <v>1</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
@@ -1588,16 +1588,16 @@
         <v>1</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
@@ -1608,7 +1608,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="5"/>
       <c r="B37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1625,13 +1625,13 @@
         <v>1</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="7"/>
@@ -1643,7 +1643,7 @@
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
       <c r="B39" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1660,16 +1660,16 @@
         <v>1</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
@@ -1683,16 +1683,16 @@
         <v>1</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
@@ -1706,13 +1706,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="7"/>

</xml_diff>

<commit_message>
MIC supply filter fix.
</commit_message>
<xml_diff>
--- a/kk_sem_ultrahang_hw_bom.xlsx
+++ b/kk_sem_ultrahang_hw_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balazs\Documents\git\kk-sem-ultrahang-hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A82E88A-E83E-4E9B-9430-A3776767E203}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D4FFA0-FB58-4758-81E7-C1D4697C6418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{81796AB7-53DE-480E-97DB-C5D69645F3D3}"/>
   </bookViews>
@@ -297,33 +297,12 @@
     <t>INDUCTOR</t>
   </si>
   <si>
-    <t>1k ferrite bead</t>
-  </si>
-  <si>
     <t>FB1, FB2</t>
   </si>
   <si>
     <t>@100MHz</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C6, C9, C10, C11, C12, C13</t>
-  </si>
-  <si>
-    <t>C7, C8, C14, C15, C16, C19, C21, C25</t>
-  </si>
-  <si>
-    <t>C17, C18</t>
-  </si>
-  <si>
-    <t>C20, C24, C26</t>
-  </si>
-  <si>
-    <t>C22</t>
-  </si>
-  <si>
-    <t>C23</t>
-  </si>
-  <si>
     <t>R1, R12</t>
   </si>
   <si>
@@ -349,12 +328,36 @@
   </si>
   <si>
     <t>390</t>
+  </si>
+  <si>
+    <t>600 ferrite bead</t>
+  </si>
+  <si>
+    <t>C1, C2, C3, C4, C5, C6, C10, C11, C12, C13, C14</t>
+  </si>
+  <si>
+    <t>C7, C23</t>
+  </si>
+  <si>
+    <t>C8, C9, C15, C16, C17, C20, C22, C26</t>
+  </si>
+  <si>
+    <t>C18, C19</t>
+  </si>
+  <si>
+    <t>C21, C25, C27</t>
+  </si>
+  <si>
+    <t>C24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="#,##0\ &quot;Ft&quot;"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -467,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -483,6 +486,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -827,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{291FD758-5D1A-4BF4-8D9E-99A6B71ACB77}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -838,7 +843,7 @@
     <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.53125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.06640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -896,7 +901,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
@@ -917,7 +922,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="I3" s="12"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
@@ -938,7 +943,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
@@ -959,7 +964,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
+      <c r="I5" s="12"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
@@ -973,7 +978,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="I6" s="11"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
@@ -994,7 +999,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
@@ -1015,7 +1020,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.45">
@@ -1029,7 +1034,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:13" ht="14.65" customHeight="1" x14ac:dyDescent="0.45">
@@ -1050,7 +1055,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
@@ -1064,7 +1069,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="11"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
@@ -1073,21 +1078,21 @@
         <v>2</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
@@ -1101,7 +1106,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="11"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
@@ -1116,7 +1121,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>52</v>
@@ -1124,22 +1129,22 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
-        <f>$M$1*8</f>
-        <v>8</v>
+        <f>$M$1*2</f>
+        <v>2</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>23</v>
@@ -1147,76 +1152,76 @@
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
-        <f>$M$1*2</f>
-        <v>2</v>
+        <f>$M$1*8</f>
+        <v>8</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
-        <f>$M$1*3</f>
-        <v>3</v>
+        <f>$M$1*2</f>
+        <v>2</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
-        <f>$M$1*1</f>
-        <v>1</v>
+        <f>$M$1*3</f>
+        <v>3</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -1231,7 +1236,7 @@
         <v>22</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>23</v>
@@ -1239,7 +1244,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
@@ -1253,7 +1258,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="I20" s="11"/>
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
@@ -1268,7 +1273,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>29</v>
@@ -1276,7 +1281,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
@@ -1299,7 +1304,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
@@ -1322,7 +1327,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="I23" s="12"/>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
@@ -1345,7 +1350,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="I24" s="12"/>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
@@ -1368,7 +1373,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="I25" s="12"/>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
@@ -1391,7 +1396,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
+      <c r="I26" s="12"/>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
@@ -1414,7 +1419,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="I27" s="12"/>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
@@ -1437,7 +1442,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
+      <c r="I28" s="12"/>
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
@@ -1460,7 +1465,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="I29" s="12"/>
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
@@ -1475,7 +1480,7 @@
         <v>22</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>29</v>
@@ -1483,7 +1488,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="I30" s="12"/>
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
@@ -1498,7 +1503,7 @@
         <v>22</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>29</v>
@@ -1506,7 +1511,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
+      <c r="I31" s="12"/>
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
@@ -1521,7 +1526,7 @@
         <v>22</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>29</v>
@@ -1529,7 +1534,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
+      <c r="I32" s="12"/>
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
@@ -1544,7 +1549,7 @@
         <v>22</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>29</v>
@@ -1552,7 +1557,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
+      <c r="I33" s="12"/>
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
@@ -1575,7 +1580,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="I34" s="12"/>
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
@@ -1590,7 +1595,7 @@
         <v>22</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>29</v>
@@ -1598,7 +1603,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
+      <c r="I35" s="12"/>
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
@@ -1613,7 +1618,7 @@
         <v>22</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>29</v>
@@ -1621,7 +1626,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
+      <c r="I36" s="12"/>
       <c r="J36" s="4"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
@@ -1630,13 +1635,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>31</v>
@@ -1644,7 +1649,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
+      <c r="I37" s="12"/>
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
@@ -1667,7 +1672,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
+      <c r="I38" s="12"/>
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
@@ -1681,7 +1686,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
+      <c r="I39" s="11"/>
       <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
@@ -1702,7 +1707,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
+      <c r="I40" s="12"/>
       <c r="J40" s="4"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
@@ -1716,7 +1721,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
+      <c r="I41" s="11"/>
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
@@ -1739,7 +1744,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
+      <c r="I42" s="12"/>
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
@@ -1762,7 +1767,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="I43" s="12"/>
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
@@ -1783,8 +1788,14 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="I44" s="12"/>
       <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I45" s="11">
+        <f>SUM(I2:I44)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1805,7 +1816,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J5 J7:J8 J42:J44 J14:J19 J21:J38 J40 J10 J12" xr:uid="{F7F205F8-AFB0-4666-BB5B-48C0AB512A47}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J5 J7:J8 J42:J44 J21:J38 J40 J10 J12 J14:J19" xr:uid="{F7F205F8-AFB0-4666-BB5B-48C0AB512A47}">
       <formula1>"Ordered,Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>